<commit_message>
Add Generate pdf & excel files from situation-cloture function
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_2022-03.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_2022-03.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -585,9 +585,993 @@
         <v>33750</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C6" t="str">
+        <v>25689432</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Anas test</v>
+      </c>
+      <c r="E6" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F6" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C7" t="str">
+        <v>ks123456</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Yassine test</v>
+      </c>
+      <c r="E7" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F7" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G7">
+        <v>75000</v>
+      </c>
+      <c r="H7">
+        <v>25000</v>
+      </c>
+      <c r="I7">
+        <v>15</v>
+      </c>
+      <c r="J7">
+        <v>7500</v>
+      </c>
+      <c r="K7">
+        <v>3750</v>
+      </c>
+      <c r="L7">
+        <v>25000</v>
+      </c>
+      <c r="M7">
+        <v>67500</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C8" t="str">
+        <v>ks12</v>
+      </c>
+      <c r="D8" t="str">
+        <v>ahmed test</v>
+      </c>
+      <c r="E8" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F8" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G8">
+        <v>37500</v>
+      </c>
+      <c r="H8">
+        <v>12500</v>
+      </c>
+      <c r="I8">
+        <v>15</v>
+      </c>
+      <c r="J8">
+        <v>3750</v>
+      </c>
+      <c r="K8">
+        <v>1875</v>
+      </c>
+      <c r="L8">
+        <v>12500</v>
+      </c>
+      <c r="M8">
+        <v>33750</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C9" t="str">
+        <v>123465</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Youssef test</v>
+      </c>
+      <c r="E9" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F9" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G9">
+        <v>37500</v>
+      </c>
+      <c r="H9">
+        <v>12500</v>
+      </c>
+      <c r="I9">
+        <v>15</v>
+      </c>
+      <c r="J9">
+        <v>3750</v>
+      </c>
+      <c r="K9">
+        <v>1875</v>
+      </c>
+      <c r="L9">
+        <v>12500</v>
+      </c>
+      <c r="M9">
+        <v>33750</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C10" t="str">
+        <v>25689432</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Anas test</v>
+      </c>
+      <c r="E10" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F10" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C11" t="str">
+        <v>ks123456</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Yassine test</v>
+      </c>
+      <c r="E11" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F11" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G11">
+        <v>75000</v>
+      </c>
+      <c r="H11">
+        <v>25000</v>
+      </c>
+      <c r="I11">
+        <v>15</v>
+      </c>
+      <c r="J11">
+        <v>7500</v>
+      </c>
+      <c r="K11">
+        <v>3750</v>
+      </c>
+      <c r="L11">
+        <v>25000</v>
+      </c>
+      <c r="M11">
+        <v>67500</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C12" t="str">
+        <v>ks12</v>
+      </c>
+      <c r="D12" t="str">
+        <v>ahmed test</v>
+      </c>
+      <c r="E12" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F12" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G12">
+        <v>37500</v>
+      </c>
+      <c r="H12">
+        <v>12500</v>
+      </c>
+      <c r="I12">
+        <v>15</v>
+      </c>
+      <c r="J12">
+        <v>3750</v>
+      </c>
+      <c r="K12">
+        <v>1875</v>
+      </c>
+      <c r="L12">
+        <v>12500</v>
+      </c>
+      <c r="M12">
+        <v>33750</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C13" t="str">
+        <v>123465</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Youssef test</v>
+      </c>
+      <c r="E13" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F13" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G13">
+        <v>37500</v>
+      </c>
+      <c r="H13">
+        <v>12500</v>
+      </c>
+      <c r="I13">
+        <v>15</v>
+      </c>
+      <c r="J13">
+        <v>3750</v>
+      </c>
+      <c r="K13">
+        <v>1875</v>
+      </c>
+      <c r="L13">
+        <v>12500</v>
+      </c>
+      <c r="M13">
+        <v>33750</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C14" t="str">
+        <v>25689432</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Anas test</v>
+      </c>
+      <c r="E14" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F14" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C15" t="str">
+        <v>ks123456</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Yassine test</v>
+      </c>
+      <c r="E15" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F15" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G15">
+        <v>75000</v>
+      </c>
+      <c r="H15">
+        <v>25000</v>
+      </c>
+      <c r="I15">
+        <v>15</v>
+      </c>
+      <c r="J15">
+        <v>7500</v>
+      </c>
+      <c r="K15">
+        <v>3750</v>
+      </c>
+      <c r="L15">
+        <v>25000</v>
+      </c>
+      <c r="M15">
+        <v>67500</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C16" t="str">
+        <v>ks12</v>
+      </c>
+      <c r="D16" t="str">
+        <v>ahmed test</v>
+      </c>
+      <c r="E16" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F16" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G16">
+        <v>37500</v>
+      </c>
+      <c r="H16">
+        <v>12500</v>
+      </c>
+      <c r="I16">
+        <v>15</v>
+      </c>
+      <c r="J16">
+        <v>3750</v>
+      </c>
+      <c r="K16">
+        <v>1875</v>
+      </c>
+      <c r="L16">
+        <v>12500</v>
+      </c>
+      <c r="M16">
+        <v>33750</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C17" t="str">
+        <v>123465</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Youssef test</v>
+      </c>
+      <c r="E17" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F17" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G17">
+        <v>37500</v>
+      </c>
+      <c r="H17">
+        <v>12500</v>
+      </c>
+      <c r="I17">
+        <v>15</v>
+      </c>
+      <c r="J17">
+        <v>3750</v>
+      </c>
+      <c r="K17">
+        <v>1875</v>
+      </c>
+      <c r="L17">
+        <v>12500</v>
+      </c>
+      <c r="M17">
+        <v>33750</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C18" t="str">
+        <v>25689432</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Anas test</v>
+      </c>
+      <c r="E18" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F18" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C19" t="str">
+        <v>ks123456</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Yassine test</v>
+      </c>
+      <c r="E19" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F19" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G19">
+        <v>75000</v>
+      </c>
+      <c r="H19">
+        <v>25000</v>
+      </c>
+      <c r="I19">
+        <v>15</v>
+      </c>
+      <c r="J19">
+        <v>7500</v>
+      </c>
+      <c r="K19">
+        <v>3750</v>
+      </c>
+      <c r="L19">
+        <v>25000</v>
+      </c>
+      <c r="M19">
+        <v>67500</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C20" t="str">
+        <v>ks12</v>
+      </c>
+      <c r="D20" t="str">
+        <v>ahmed test</v>
+      </c>
+      <c r="E20" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F20" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G20">
+        <v>37500</v>
+      </c>
+      <c r="H20">
+        <v>12500</v>
+      </c>
+      <c r="I20">
+        <v>15</v>
+      </c>
+      <c r="J20">
+        <v>3750</v>
+      </c>
+      <c r="K20">
+        <v>1875</v>
+      </c>
+      <c r="L20">
+        <v>12500</v>
+      </c>
+      <c r="M20">
+        <v>33750</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C21" t="str">
+        <v>123465</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Youssef test</v>
+      </c>
+      <c r="E21" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F21" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G21">
+        <v>37500</v>
+      </c>
+      <c r="H21">
+        <v>12500</v>
+      </c>
+      <c r="I21">
+        <v>15</v>
+      </c>
+      <c r="J21">
+        <v>3750</v>
+      </c>
+      <c r="K21">
+        <v>1875</v>
+      </c>
+      <c r="L21">
+        <v>12500</v>
+      </c>
+      <c r="M21">
+        <v>33750</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C22" t="str">
+        <v>25689432</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Anas test</v>
+      </c>
+      <c r="E22" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F22" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C23" t="str">
+        <v>ks123456</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Yassine test</v>
+      </c>
+      <c r="E23" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F23" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G23">
+        <v>75000</v>
+      </c>
+      <c r="H23">
+        <v>25000</v>
+      </c>
+      <c r="I23">
+        <v>15</v>
+      </c>
+      <c r="J23">
+        <v>7500</v>
+      </c>
+      <c r="K23">
+        <v>3750</v>
+      </c>
+      <c r="L23">
+        <v>25000</v>
+      </c>
+      <c r="M23">
+        <v>67500</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C24" t="str">
+        <v>ks12</v>
+      </c>
+      <c r="D24" t="str">
+        <v>ahmed test</v>
+      </c>
+      <c r="E24" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F24" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G24">
+        <v>37500</v>
+      </c>
+      <c r="H24">
+        <v>12500</v>
+      </c>
+      <c r="I24">
+        <v>15</v>
+      </c>
+      <c r="J24">
+        <v>3750</v>
+      </c>
+      <c r="K24">
+        <v>1875</v>
+      </c>
+      <c r="L24">
+        <v>12500</v>
+      </c>
+      <c r="M24">
+        <v>33750</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C25" t="str">
+        <v>123465</v>
+      </c>
+      <c r="D25" t="str">
+        <v>Youssef test</v>
+      </c>
+      <c r="E25" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F25" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G25">
+        <v>37500</v>
+      </c>
+      <c r="H25">
+        <v>12500</v>
+      </c>
+      <c r="I25">
+        <v>15</v>
+      </c>
+      <c r="J25">
+        <v>3750</v>
+      </c>
+      <c r="K25">
+        <v>1875</v>
+      </c>
+      <c r="L25">
+        <v>12500</v>
+      </c>
+      <c r="M25">
+        <v>33750</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C26" t="str">
+        <v>25689432</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Anas test</v>
+      </c>
+      <c r="E26" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F26" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C27" t="str">
+        <v>ks123456</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Yassine test</v>
+      </c>
+      <c r="E27" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F27" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G27">
+        <v>75000</v>
+      </c>
+      <c r="H27">
+        <v>25000</v>
+      </c>
+      <c r="I27">
+        <v>15</v>
+      </c>
+      <c r="J27">
+        <v>7500</v>
+      </c>
+      <c r="K27">
+        <v>3750</v>
+      </c>
+      <c r="L27">
+        <v>25000</v>
+      </c>
+      <c r="M27">
+        <v>67500</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C28" t="str">
+        <v>ks12</v>
+      </c>
+      <c r="D28" t="str">
+        <v>ahmed test</v>
+      </c>
+      <c r="E28" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F28" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G28">
+        <v>37500</v>
+      </c>
+      <c r="H28">
+        <v>12500</v>
+      </c>
+      <c r="I28">
+        <v>15</v>
+      </c>
+      <c r="J28">
+        <v>3750</v>
+      </c>
+      <c r="K28">
+        <v>1875</v>
+      </c>
+      <c r="L28">
+        <v>12500</v>
+      </c>
+      <c r="M28">
+        <v>33750</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>001/DR 1</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C29" t="str">
+        <v>123465</v>
+      </c>
+      <c r="D29" t="str">
+        <v>Youssef test</v>
+      </c>
+      <c r="E29" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F29" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G29">
+        <v>37500</v>
+      </c>
+      <c r="H29">
+        <v>12500</v>
+      </c>
+      <c r="I29">
+        <v>15</v>
+      </c>
+      <c r="J29">
+        <v>3750</v>
+      </c>
+      <c r="K29">
+        <v>1875</v>
+      </c>
+      <c r="L29">
+        <v>12500</v>
+      </c>
+      <c r="M29">
+        <v>33750</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M29"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>